<commit_message>
Fixed plot formatting, relabeled contact type and surface chemistry.
Included final experimental data and related statistics.
</commit_message>
<xml_diff>
--- a/Data/gecko_comparison.xlsx
+++ b/Data/gecko_comparison.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Documents\paper-underwater_adhesion\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adwait\Desktop\MPIP\Documents\paper-underwater_adhesion\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,10 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$9</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="12">
   <si>
     <t>Substrate</t>
   </si>
@@ -65,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,10 +414,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>17</v>
+        <v>40.299999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -425,94 +428,94 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>5.5</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>27</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>24</v>
+        <v>33.85</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>37.99</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>17.5</v>
+        <v>40.78</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>38.97</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9">
-        <v>7.5</v>
+        <v>40.06</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -523,10 +526,10 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>40.299999999999997</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -537,94 +540,318 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>12.4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12">
-        <v>20.3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13">
-        <v>33.85</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>37.99</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15">
-        <v>40.78</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16">
-        <v>38.97</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>6</v>
       </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17">
-        <v>40.06</v>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>21.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>